<commit_message>
A little index and a lot of Lecture A
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>Time</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Thursday</t>
+  </si>
+  <si>
+    <t>See todo</t>
   </si>
 </sst>
 </file>
@@ -745,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -886,6 +889,7 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1440,7 +1444,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1501,6 +1505,12 @@
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="46"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">

</xml_diff>